<commit_message>
added toggle of player names
</commit_message>
<xml_diff>
--- a/model/Squoids_data/Squoids floor builder 20180106.xlsx
+++ b/model/Squoids_data/Squoids floor builder 20180106.xlsx
@@ -35,7 +35,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Tiles!$C$1:$C$65</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2252,18 +2251,32 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="50">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2306,314 +2319,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5677,12 +5382,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y26">
-    <cfRule type="expression" dxfId="91" priority="2">
+    <cfRule type="expression" dxfId="49" priority="2">
       <formula>AND(COLUMN()&lt;=$B$27,ROW()&lt;=$B$28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z26">
-    <cfRule type="cellIs" dxfId="90" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7410,12 +7115,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="63" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="62" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9143,22 +8848,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="61" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="60" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="59" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND(COLUMN()&lt;=$B$27,ROW()&lt;=$B$28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="58" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10886,12 +10591,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="57" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="56" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12619,12 +12324,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="55" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="54" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14350,12 +14055,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="53" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="52" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14534,7 +14239,7 @@
         <v xml:space="preserve">~~~~~~~~~~~~~~~~~~~ </v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AB25" si="1">"'"&amp;AA2&amp;"',"</f>
+        <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
         <v>'~~~~~~~~~~~~~~~~~~~ ',</v>
       </c>
     </row>
@@ -16203,12 +15908,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="47" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="46" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16222,7 +15927,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16387,7 +16092,7 @@
         <v xml:space="preserve">                    </v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AB25" si="1">"'"&amp;AA2&amp;"',"</f>
+        <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
         <v>'                    ',</v>
       </c>
     </row>
@@ -16554,7 +16259,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>5</v>
@@ -16563,13 +16268,13 @@
         <v>6</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>13</v>
+        <v>258</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>61</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>258</v>
+        <v>12</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>6</v>
@@ -16621,11 +16326,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">+#+ (*\             </v>
+        <v xml:space="preserve">+H+ \*)             </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'+#+ (*\             ',</v>
+        <v>'+H+ \*)             ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -17052,7 +16757,7 @@
         <v>5</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>5</v>
@@ -17095,11 +16800,11 @@
       </c>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">        +#+  *** ***</v>
+        <v xml:space="preserve">        +H+  *** ***</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'        +#+  *** ***',</v>
+        <v>'        +H+  *** ***',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -17474,7 +17179,7 @@
         <v>61</v>
       </c>
       <c r="S16" s="12" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="T16" s="12" t="s">
         <v>61</v>
@@ -17490,11 +17195,11 @@
       </c>
       <c r="AA16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">        (*\  (*\ ***</v>
+        <v xml:space="preserve">        (*\  (*\ *+*</v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="1"/>
-        <v>'        (*\  (*\ ***',</v>
+        <v>'        (*\  (*\ *+*',</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -18056,12 +17761,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="45" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="44" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18240,7 +17945,7 @@
         <v xml:space="preserve">                    </v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AB25" si="1">"'"&amp;AA2&amp;"',"</f>
+        <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
         <v>'                    ',</v>
       </c>
     </row>
@@ -19909,12 +19614,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="35" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="34" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22328,22 +22033,22 @@
     <sortCondition ref="B2:B67"/>
   </sortState>
   <conditionalFormatting sqref="D1:D31 D33:D1048576">
-    <cfRule type="cellIs" dxfId="51" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 K33:K77">
-    <cfRule type="cellIs" dxfId="50" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22522,7 +22227,7 @@
         <v xml:space="preserve">                    </v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AB25" si="1">"'"&amp;AA2&amp;"',"</f>
+        <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
         <v>'                    ',</v>
       </c>
     </row>
@@ -24191,12 +23896,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="89" priority="2">
+    <cfRule type="expression" dxfId="47" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="88" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25924,22 +25629,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="87" priority="4">
+    <cfRule type="expression" dxfId="45" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="86" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="85" priority="2">
+    <cfRule type="expression" dxfId="43" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="84" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27665,22 +27370,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20 A19">
-    <cfRule type="expression" dxfId="83" priority="4">
+    <cfRule type="expression" dxfId="41" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20 A19">
-    <cfRule type="cellIs" dxfId="82" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20 A1:T2 A3:A18 B3:T20">
-    <cfRule type="expression" dxfId="81" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20 A1:T2 A3:A18 B3:T20">
-    <cfRule type="cellIs" dxfId="80" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29412,22 +29117,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="79" priority="4">
+    <cfRule type="expression" dxfId="37" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="78" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="77" priority="2">
+    <cfRule type="expression" dxfId="35" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="76" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31155,22 +30860,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="75" priority="4">
+    <cfRule type="expression" dxfId="33" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="74" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="73" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="72" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32898,22 +32603,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="71" priority="4">
+    <cfRule type="expression" dxfId="29" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="70" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="69" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="68" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34641,12 +34346,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="67" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="66" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36374,12 +36079,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="65" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="64" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>